<commit_message>
Updated helper mapping spreadsheet
</commit_message>
<xml_diff>
--- a/docs/TOCHelper-KingsFieldMappings.xlsx
+++ b/docs/TOCHelper-KingsFieldMappings.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Mapping from Word Doc" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,15 +17,17 @@
     <definedName function="false" hidden="true" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Helper Fields'!$A$3:$E$58</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area" vbProcedure="false">'Helper Fields'!$A$3:$E$47</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0" vbProcedure="false">'Helper Fields'!$A$3:$E$47</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Helper Fields'!$A$3:$E$47</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase" vbProcedure="false">'Helper Fields'!$A$3:$E$58</definedName>
     <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Helper Fields'!$A$3:$E$58</definedName>
+    <definedName function="false" hidden="false" localSheetId="1" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Helper Fields'!$A$3:$E$58</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="789" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="797" uniqueCount="359">
   <si>
     <t>KEY</t>
   </si>
@@ -1112,7 +1114,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YYYY\ HH:MM"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1164,6 +1166,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFC5000B"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1207,7 +1216,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1249,10 +1258,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="4" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="7" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1265,6 +1278,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FFC5000B"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFC0C0C0"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -1279,8 +1352,8 @@
   </sheetPr>
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A75" activeCellId="0" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2130,7 +2203,7 @@
   </sheetPr>
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A73" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B99" activeCellId="0" sqref="B99"/>
     </sheetView>
   </sheetViews>
@@ -4211,10 +4284,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C43"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4576,20 +4649,26 @@
         <v>330</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
         <v>345</v>
       </c>
-      <c r="B35" s="0" t="s">
+      <c r="B35" s="12" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C35" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
         <v>347</v>
       </c>
-      <c r="B36" s="0" t="s">
+      <c r="B36" s="12" t="s">
         <v>346</v>
+      </c>
+      <c r="C36" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4667,6 +4746,28 @@
       </c>
       <c r="C43" s="1" t="s">
         <v>358</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B44" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C44" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="B45" s="12" t="s">
+        <v>346</v>
+      </c>
+      <c r="C45" s="12" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>